<commit_message>
del and new file
</commit_message>
<xml_diff>
--- a/ab.xlsx
+++ b/ab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRATIBHA\Documents\new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E5EA39-8F48-4875-9161-EC7B789A0B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAC1AD9-7FA5-461A-99AE-55572E875C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="2">
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>abh</t>
   </si>
 </sst>
 </file>
@@ -345,160 +348,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>2</v>
+      <c r="C2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>3</v>
+      <c r="C3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>4</v>
+      <c r="C4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>